<commit_message>
#7 Add security headers interceptor and transformed input sanitizer to an interceptor
</commit_message>
<xml_diff>
--- a/Deliverables/Documentation/P2_sprint2/v4-ASVS-checklist-en_sprint_2.xlsx
+++ b/Deliverables/Documentation/P2_sprint2/v4-ASVS-checklist-en_sprint_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Fernandes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISEP\repos\desofs2024_M1A_1\Deliverables\Documentation\P2_sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEA8438-5DE0-4E3D-97FD-F4161E0DDA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816678C4-DA9E-4C76-A9B6-AF54E8B055EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="831" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="831" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="875">
   <si>
     <t>Security Category</t>
   </si>
@@ -2704,6 +2704,12 @@
   </si>
   <si>
     <t>README_User</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.config.SecurityHeadersInterceptor</t>
+  </si>
+  <si>
+    <t>This interceptor guarantee that all response headers contains security headers</t>
   </si>
 </sst>
 </file>
@@ -3505,7 +3511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3888,6 +3894,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4713,7 +4722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -6792,8 +6801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -7175,7 +7184,7 @@
       <c r="I14" s="125"/>
       <c r="J14" s="126"/>
     </row>
-    <row r="15" spans="1:10" ht="31.5">
+    <row r="15" spans="1:10" ht="32.25" thickBot="1">
       <c r="A15" s="139"/>
       <c r="B15" s="62" t="s">
         <v>662</v>
@@ -7196,10 +7205,10 @@
       <c r="H15" s="125" t="s">
         <v>726</v>
       </c>
-      <c r="I15" s="125"/>
+      <c r="I15" s="141"/>
       <c r="J15" s="126"/>
     </row>
-    <row r="16" spans="1:10" ht="48" customHeight="1">
+    <row r="16" spans="1:10" ht="48" customHeight="1" thickBot="1">
       <c r="A16" s="139" t="s">
         <v>664</v>
       </c>
@@ -7220,12 +7229,14 @@
         <v>26</v>
       </c>
       <c r="H16" s="125" t="s">
-        <v>726</v>
-      </c>
-      <c r="I16" s="125"/>
+        <v>873</v>
+      </c>
+      <c r="I16" s="125" t="s">
+        <v>874</v>
+      </c>
       <c r="J16" s="126"/>
     </row>
-    <row r="17" spans="1:10" ht="31.5">
+    <row r="17" spans="1:10" ht="48" thickBot="1">
       <c r="A17" s="139"/>
       <c r="B17" s="62" t="s">
         <v>667</v>
@@ -7244,12 +7255,14 @@
         <v>26</v>
       </c>
       <c r="H17" s="125" t="s">
-        <v>726</v>
-      </c>
-      <c r="I17" s="125"/>
+        <v>873</v>
+      </c>
+      <c r="I17" s="125" t="s">
+        <v>874</v>
+      </c>
       <c r="J17" s="126"/>
     </row>
-    <row r="18" spans="1:10" ht="31.5">
+    <row r="18" spans="1:10" ht="47.25">
       <c r="A18" s="139"/>
       <c r="B18" s="62" t="s">
         <v>669</v>
@@ -7268,12 +7281,14 @@
         <v>26</v>
       </c>
       <c r="H18" s="125" t="s">
-        <v>726</v>
-      </c>
-      <c r="I18" s="125"/>
+        <v>873</v>
+      </c>
+      <c r="I18" s="125" t="s">
+        <v>874</v>
+      </c>
       <c r="J18" s="126"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75">
+    <row r="19" spans="1:10" ht="47.25">
       <c r="A19" s="139"/>
       <c r="B19" s="62" t="s">
         <v>671</v>
@@ -7292,12 +7307,14 @@
         <v>26</v>
       </c>
       <c r="H19" s="125" t="s">
-        <v>726</v>
-      </c>
-      <c r="I19" s="125"/>
+        <v>873</v>
+      </c>
+      <c r="I19" s="125" t="s">
+        <v>874</v>
+      </c>
       <c r="J19" s="126"/>
     </row>
-    <row r="20" spans="1:10" ht="31.5">
+    <row r="20" spans="1:10" ht="47.25">
       <c r="A20" s="139"/>
       <c r="B20" s="62" t="s">
         <v>673</v>
@@ -7316,12 +7333,14 @@
         <v>26</v>
       </c>
       <c r="H20" s="125" t="s">
-        <v>726</v>
-      </c>
-      <c r="I20" s="125"/>
+        <v>873</v>
+      </c>
+      <c r="I20" s="125" t="s">
+        <v>874</v>
+      </c>
       <c r="J20" s="126"/>
     </row>
-    <row r="21" spans="1:10" ht="31.5">
+    <row r="21" spans="1:10" ht="47.25">
       <c r="A21" s="139"/>
       <c r="B21" s="62" t="s">
         <v>675</v>
@@ -7340,9 +7359,11 @@
         <v>26</v>
       </c>
       <c r="H21" s="125" t="s">
-        <v>726</v>
-      </c>
-      <c r="I21" s="125"/>
+        <v>873</v>
+      </c>
+      <c r="I21" s="125" t="s">
+        <v>874</v>
+      </c>
       <c r="J21" s="126"/>
     </row>
     <row r="22" spans="1:10" ht="63">
@@ -7364,9 +7385,11 @@
         <v>26</v>
       </c>
       <c r="H22" s="125" t="s">
-        <v>726</v>
-      </c>
-      <c r="I22" s="125"/>
+        <v>873</v>
+      </c>
+      <c r="I22" s="125" t="s">
+        <v>874</v>
+      </c>
       <c r="J22" s="126"/>
     </row>
     <row r="23" spans="1:10" ht="48" customHeight="1">
@@ -7498,7 +7521,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -7510,7 +7533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
@@ -8704,17 +8727,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -10303,16 +10326,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="A45:A51"/>
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -13661,6 +13684,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="caec8013-4252-46d5-9263-a99cc59dead2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d77a0e16-36e2-4619-a824-6737dea303d4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E2F6ACCA1C4E9E429EC0979D7AA69E5C" ma:contentTypeVersion="14" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="2bb008ca7a1b4eda16785ddef8185b41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="caec8013-4252-46d5-9263-a99cc59dead2" xmlns:ns3="d77a0e16-36e2-4619-a824-6737dea303d4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3d1966398a198bcd33f0542821d602e" ns2:_="" ns3:_="">
     <xsd:import namespace="caec8013-4252-46d5-9263-a99cc59dead2"/>
@@ -13889,17 +13923,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="caec8013-4252-46d5-9263-a99cc59dead2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d77a0e16-36e2-4619-a824-6737dea303d4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1115CF8-E078-4757-AB4D-549A55AF833E}">
   <ds:schemaRefs>
@@ -13909,6 +13932,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB94848C-75E5-4594-8307-209BB5BE433B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="caec8013-4252-46d5-9263-a99cc59dead2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d77a0e16-36e2-4619-a824-6737dea303d4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{088014DA-7408-4969-8EBB-5375B357E254}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13925,21 +13965,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB94848C-75E5-4594-8307-209BB5BE433B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="caec8013-4252-46d5-9263-a99cc59dead2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="d77a0e16-36e2-4619-a824-6737dea303d4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
#1 ASVS - Final documentation
</commit_message>
<xml_diff>
--- a/Deliverables/Documentation/P2_sprint2/v4-ASVS-checklist-en_sprint_2.xlsx
+++ b/Deliverables/Documentation/P2_sprint2/v4-ASVS-checklist-en_sprint_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISEP\repos\desofs2024_M1A_1\Deliverables\Documentation\P2_sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myisepipp.sharepoint.com/teams/Abelhudos-ISEP365Group/Shared Documents/DESOFS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816678C4-DA9E-4C76-A9B6-AF54E8B055EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{816678C4-DA9E-4C76-A9B6-AF54E8B055EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{425A4772-6EC3-4429-BFEB-15F2B4885345}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="831" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21240" tabRatio="831" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="893">
   <si>
     <t>Security Category</t>
   </si>
@@ -2265,9 +2265,6 @@
     <t>This method is a one read only method</t>
   </si>
   <si>
-    <t>Not implemented yet</t>
-  </si>
-  <si>
     <t>org.springframework.security.crypto.password.PasswordEncoder.encode(CharSequence)</t>
   </si>
   <si>
@@ -2331,9 +2328,6 @@
     <t>All of endpoints are restricted for authenticated user role.</t>
   </si>
   <si>
-    <t>Not Implement yet</t>
-  </si>
-  <si>
     <t>Passwords are encoded using Spring Security's PasswordEncoder.</t>
   </si>
   <si>
@@ -2454,9 +2448,6 @@
     <t>Provides CI/CD workflow, build instructions, and automation tools.</t>
   </si>
   <si>
-    <t>pipeline.yml, README_P2_Sprint_1.md</t>
-  </si>
-  <si>
     <t>GitHub Actions</t>
   </si>
   <si>
@@ -2469,9 +2460,6 @@
     <t>Maven, GitHub Actions</t>
   </si>
   <si>
-    <t>Not Implemented yet</t>
-  </si>
-  <si>
     <t>Dependabot alerts, Dependency Checker</t>
   </si>
   <si>
@@ -2490,9 +2478,6 @@
     <t>SecurityConfig shows us what each user can acces</t>
   </si>
   <si>
-    <t>Not Implemented Yet</t>
-  </si>
-  <si>
     <t>pipeline.yml is the configuration file that is executed inside GitHub Actions</t>
   </si>
   <si>
@@ -2535,9 +2520,6 @@
     <t>Ensures sequential step order processing using service layer validation.</t>
   </si>
   <si>
-    <t>Implements anti-automation controls using CAPTCHA and rate limiting.</t>
-  </si>
-  <si>
     <t>Uses threat modeling to identify and enforce business logic limits.</t>
   </si>
   <si>
@@ -2547,9 +2529,6 @@
     <t>Configurable alerting for detected automated attacks or unusual activity.</t>
   </si>
   <si>
-    <t>Not implement yet</t>
-  </si>
-  <si>
     <t>Readme.md -&gt; Data Flow Diagram</t>
   </si>
   <si>
@@ -2685,9 +2664,6 @@
     <t>Application deployments use containerization and network isolation to enhance security and prevent attacks.</t>
   </si>
   <si>
-    <t>build_deploy.puml</t>
-  </si>
-  <si>
     <t>pt.isep.desofs.m1a.g1.model.user.Password</t>
   </si>
   <si>
@@ -2710,6 +2686,84 @@
   </si>
   <si>
     <t>This interceptor guarantee that all response headers contains security headers</t>
+  </si>
+  <si>
+    <t>Post handler nterceptor</t>
+  </si>
+  <si>
+    <t>Validate password</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.config.SecurityHeadersInterceptor, pt.isep.desofs.m1a.g1.config.InputSanitizerInterceptor, pt.isep.desofs.m1a.g1.config.RateLimitInterceptor</t>
+  </si>
+  <si>
+    <t>Interceptor validate this constraints</t>
+  </si>
+  <si>
+    <t>org.springframework.web.servlet.config.annotation.WebMvcConfigurer</t>
+  </si>
+  <si>
+    <t>Only permit frontend endpoint for development</t>
+  </si>
+  <si>
+    <t>build.puml and release.puml</t>
+  </si>
+  <si>
+    <t>2FA implementation in backend and frontend</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.service.TwoFactorAuthService, two-factor-auth component</t>
+  </si>
+  <si>
+    <t>The InputSanitizer class ensures that HTML cannot go through</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.config.RateLimitInterceptor</t>
+  </si>
+  <si>
+    <t>Manual Code review</t>
+  </si>
+  <si>
+    <t>It limits the request based on a bucket</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.config.MonitoringInterceptor</t>
+  </si>
+  <si>
+    <t>Monitoring is saved in database.</t>
+  </si>
+  <si>
+    <t>Only contains token</t>
+  </si>
+  <si>
+    <t>Password is stored encrypted</t>
+  </si>
+  <si>
+    <t>All data is stored in the database as soon as possible</t>
+  </si>
+  <si>
+    <t>BCryptPasswordEncoder</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.service.impl.GeoLocalizationClient</t>
+  </si>
+  <si>
+    <t>Implemented in a docker container</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.config.InputSanitizerInterceptor</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.controller.DeliveryController.getDeliveryPlanPdf(String, Long)</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.config.SecurityConfig.webConfigurer().new WebMvcConfigurer() {...}.addCorsMappings(CorsRegistry)</t>
+  </si>
+  <si>
+    <t>pipeline.yml, release.yml, README_P2_Sprint_2.md</t>
+  </si>
+  <si>
+    <t>pipeline.yml, release.yml</t>
   </si>
 </sst>
 </file>
@@ -3895,7 +3949,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4165,10 +4219,10 @@
                 <c:formatCode>#\ ##0.00\ _€;\-#\ ##0.00\ _€</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>89.473684210526315</c:v>
+                  <c:v>84.210526315789465</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.666666666666657</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>60</c:v>
@@ -4177,7 +4231,7 @@
                   <c:v>88.888888888888886</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>86.666666666666671</c:v>
+                  <c:v>73.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100</c:v>
@@ -4186,10 +4240,10 @@
                   <c:v>91.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100</c:v>
+                  <c:v>81.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>90</c:v>
@@ -4201,13 +4255,13 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>69.230769230769226</c:v>
+                  <c:v>88.888888888888886</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>87.5</c:v>
+                  <c:v>83.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>81.481481481481481</c:v>
+                  <c:v>78.861788617886177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4421,6 +4475,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4722,7 +4780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -4759,7 +4817,7 @@
       </c>
       <c r="B2" s="9">
         <f>0+COUNTIF('Architecture, Design and Threat'!G2:G45,"Valid")</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="10">
         <f>COUNTIF('Architecture, Design and Threat'!G2:G45,"&lt;&gt;Not Applicable")</f>
@@ -4767,7 +4825,7 @@
       </c>
       <c r="D2" s="11">
         <f t="shared" ref="D2:D16" si="0">(B2/C2)*100</f>
-        <v>89.473684210526315</v>
+        <v>84.210526315789465</v>
       </c>
       <c r="E2" s="12"/>
     </row>
@@ -4777,15 +4835,15 @@
       </c>
       <c r="B3" s="9">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C3" s="10">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>66.666666666666657</v>
+        <v>60</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -4831,7 +4889,7 @@
       </c>
       <c r="B6" s="9">
         <f>COUNTIF('Validation, Sanitization and En'!G2:G31,"Valid")</f>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" s="10">
         <f>COUNTIF('Validation, Sanitization and En'!G2:G31,"&lt;&gt;Not Applicable")</f>
@@ -4839,7 +4897,7 @@
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>86.666666666666671</v>
+        <v>73.333333333333329</v>
       </c>
       <c r="E6" s="12"/>
     </row>
@@ -4887,15 +4945,15 @@
       </c>
       <c r="B9" s="9">
         <f>COUNTIF('Data Protection'!G2:G18,"Valid")</f>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" s="10">
         <f>COUNTIF('Data Protection'!G2:G18,"&lt;&gt;Not Applicable")</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>81.25</v>
       </c>
       <c r="E9" s="12"/>
     </row>
@@ -4905,7 +4963,7 @@
       </c>
       <c r="B10" s="9">
         <f>COUNTIF(Communication!G2:G9,"Valid")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" s="10">
         <f>COUNTIF(Communication!G2:G9,"&lt;&gt;Not Applicable")</f>
@@ -4913,7 +4971,7 @@
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="E10" s="12"/>
     </row>
@@ -4959,11 +5017,11 @@
       </c>
       <c r="B13" s="9">
         <f>COUNTIF('Files and Resources'!G2:G16,"Valid")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" s="10">
         <f>COUNTIF('Files and Resources'!G2:G16,"&lt;&gt;Not Applicable")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" s="11">
         <f t="shared" si="0"/>
@@ -4977,15 +5035,15 @@
       </c>
       <c r="B14" s="9">
         <f>COUNTIF('API and Web Service'!G2:G16,"Valid")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="10">
         <f>COUNTIF('API and Web Service'!G2:G16,"&lt;&gt;Not Applicable")</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14" s="11">
         <f t="shared" si="0"/>
-        <v>69.230769230769226</v>
+        <v>88.888888888888886</v>
       </c>
       <c r="E14" s="12"/>
     </row>
@@ -4995,7 +5053,7 @@
       </c>
       <c r="B15" s="9">
         <f>COUNTIF(Configuration!G2:G26,"Valid")</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="10">
         <f>COUNTIF(Configuration!G2:G26,"&lt;&gt;Not Applicable")</f>
@@ -5003,7 +5061,7 @@
       </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -5013,15 +5071,15 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>81.481481481481481</v>
+        <v>78.861788617886177</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -5041,7 +5099,7 @@
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -5050,14 +5108,14 @@
     <col min="2" max="2" width="8.85546875" style="25"/>
     <col min="3" max="5" width="8.85546875" style="59"/>
     <col min="6" max="6" width="88.85546875" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="25"/>
-    <col min="8" max="8" width="28.28515625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" style="25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="37.7109375" style="25" customWidth="1"/>
     <col min="11" max="1024" width="8.85546875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
+    <row r="1" spans="1:10" s="43" customFormat="1" ht="42.75" thickBot="1">
       <c r="A1" s="93" t="s">
         <v>20</v>
       </c>
@@ -5089,7 +5147,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="48" customHeight="1">
+    <row r="2" spans="1:10" ht="48" customHeight="1" thickBot="1">
       <c r="A2" s="139" t="s">
         <v>505</v>
       </c>
@@ -5109,13 +5167,13 @@
       <c r="G2" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="49" t="s">
-        <v>726</v>
-      </c>
-      <c r="I2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49" t="s">
+        <v>887</v>
+      </c>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="31.5">
+    <row r="3" spans="1:10" ht="32.25" thickBot="1">
       <c r="A3" s="139"/>
       <c r="B3" s="62" t="s">
         <v>508</v>
@@ -5133,13 +5191,13 @@
       <c r="G3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>726</v>
-      </c>
-      <c r="I3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28" t="s">
+        <v>887</v>
+      </c>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="31.5">
+    <row r="4" spans="1:10" ht="32.25" thickBot="1">
       <c r="A4" s="139"/>
       <c r="B4" s="62" t="s">
         <v>510</v>
@@ -5157,13 +5215,13 @@
       <c r="G4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="28" t="s">
-        <v>726</v>
-      </c>
-      <c r="I4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28" t="s">
+        <v>887</v>
+      </c>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" ht="63.75" customHeight="1">
+    <row r="5" spans="1:10" ht="63.75" customHeight="1" thickBot="1">
       <c r="A5" s="139" t="s">
         <v>512</v>
       </c>
@@ -5183,13 +5241,13 @@
       <c r="G5" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="28" t="s">
-        <v>726</v>
-      </c>
-      <c r="I5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28" t="s">
+        <v>887</v>
+      </c>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="63">
+    <row r="6" spans="1:10" ht="63.75" thickBot="1">
       <c r="A6" s="139"/>
       <c r="B6" s="62" t="s">
         <v>515</v>
@@ -5207,13 +5265,13 @@
       <c r="G6" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>726</v>
-      </c>
-      <c r="I6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28" t="s">
+        <v>887</v>
+      </c>
       <c r="J6" s="32"/>
     </row>
-    <row r="7" spans="1:10" ht="31.5">
+    <row r="7" spans="1:10" ht="32.25" thickBot="1">
       <c r="A7" s="139"/>
       <c r="B7" s="62" t="s">
         <v>517</v>
@@ -5231,13 +5289,13 @@
       <c r="G7" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>726</v>
-      </c>
-      <c r="I7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28" t="s">
+        <v>887</v>
+      </c>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="31.5">
+    <row r="8" spans="1:10" ht="32.25" thickBot="1">
       <c r="A8" s="139"/>
       <c r="B8" s="62" t="s">
         <v>519</v>
@@ -5253,13 +5311,15 @@
         <v>520</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>690</v>
+        <v>26</v>
       </c>
       <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
+      <c r="I8" s="28" t="s">
+        <v>887</v>
+      </c>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75">
+    <row r="9" spans="1:10" ht="16.5" thickBot="1">
       <c r="A9" s="139"/>
       <c r="B9" s="62" t="s">
         <v>521</v>
@@ -5275,10 +5335,12 @@
         <v>522</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>690</v>
+        <v>26</v>
       </c>
       <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
+      <c r="I9" s="35" t="s">
+        <v>887</v>
+      </c>
       <c r="J9" s="37"/>
     </row>
   </sheetData>
@@ -5306,7 +5368,7 @@
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -5375,13 +5437,13 @@
         <v>26</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>826</v>
+        <v>819</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="48" customHeight="1">
@@ -5405,13 +5467,13 @@
         <v>26</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>833</v>
+        <v>826</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.5">
@@ -5455,13 +5517,13 @@
         <v>26</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>832</v>
+        <v>825</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="31.5">
@@ -5482,8 +5544,8 @@
       <c r="G6" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="30" t="s">
-        <v>726</v>
+      <c r="H6" s="133" t="s">
+        <v>807</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
@@ -5507,13 +5569,13 @@
         <v>26</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>842</v>
+        <v>835</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="47.25">
@@ -5535,13 +5597,13 @@
         <v>26</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>842</v>
+        <v>835</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="48" customHeight="1">
@@ -5565,11 +5627,11 @@
         <v>26</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>837</v>
+        <v>830</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="63">
@@ -5590,8 +5652,8 @@
       <c r="G10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>726</v>
+      <c r="H10" s="133" t="s">
+        <v>886</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="31"/>
@@ -5614,10 +5676,10 @@
       <c r="G11" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="113" t="s">
-        <v>726</v>
-      </c>
-      <c r="I11" s="113"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113" t="s">
+        <v>887</v>
+      </c>
       <c r="J11" s="114"/>
     </row>
   </sheetData>
@@ -5645,7 +5707,7 @@
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -5714,10 +5776,10 @@
         <v>26</v>
       </c>
       <c r="H2" s="130" t="s">
-        <v>822</v>
+        <v>815</v>
       </c>
       <c r="I2" s="130" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="J2" s="65"/>
     </row>
@@ -5740,7 +5802,7 @@
         <v>690</v>
       </c>
       <c r="H3" s="131" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="I3" s="131"/>
       <c r="J3" s="32"/>
@@ -5764,7 +5826,7 @@
         <v>690</v>
       </c>
       <c r="H4" s="131" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="I4" s="131"/>
       <c r="J4" s="32"/>
@@ -5788,11 +5850,9 @@
         <v>26</v>
       </c>
       <c r="H5" s="131" t="s">
-        <v>820</v>
-      </c>
-      <c r="I5" s="131" t="s">
-        <v>816</v>
-      </c>
+        <v>877</v>
+      </c>
+      <c r="I5" s="131"/>
       <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="48" thickBot="1">
@@ -5814,10 +5874,10 @@
         <v>26</v>
       </c>
       <c r="H6" s="131" t="s">
-        <v>821</v>
+        <v>814</v>
       </c>
       <c r="I6" s="131" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="J6" s="32"/>
     </row>
@@ -5840,10 +5900,10 @@
         <v>690</v>
       </c>
       <c r="H7" s="131" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="I7" s="131" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="J7" s="32"/>
     </row>
@@ -5866,10 +5926,10 @@
         <v>26</v>
       </c>
       <c r="H8" s="131" t="s">
-        <v>820</v>
+        <v>877</v>
       </c>
       <c r="I8" s="131" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="J8" s="32"/>
     </row>
@@ -5892,10 +5952,10 @@
         <v>26</v>
       </c>
       <c r="H9" s="132" t="s">
-        <v>820</v>
+        <v>877</v>
       </c>
       <c r="I9" s="132" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="J9" s="37"/>
     </row>
@@ -5903,7 +5963,7 @@
   <mergeCells count="1">
     <mergeCell ref="A2:A9"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G9" xr:uid="{9E6DA540-6823-4790-9A21-4C26A7549039}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
@@ -5922,8 +5982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -6039,7 +6099,7 @@
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="1:10" ht="31.5">
+    <row r="5" spans="1:10" ht="32.25" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>570</v>
       </c>
@@ -6063,7 +6123,7 @@
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
     </row>
-    <row r="6" spans="1:10" ht="48" customHeight="1">
+    <row r="6" spans="1:10" ht="48" customHeight="1" thickBot="1">
       <c r="A6" s="139" t="s">
         <v>573</v>
       </c>
@@ -6084,12 +6144,12 @@
         <v>26</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>726</v>
+        <v>888</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
     </row>
-    <row r="7" spans="1:10" ht="31.5">
+    <row r="7" spans="1:10" ht="32.25" thickBot="1">
       <c r="A7" s="139"/>
       <c r="B7" s="62" t="s">
         <v>576</v>
@@ -6105,11 +6165,9 @@
         <v>577</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H7" s="30"/>
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
     </row>
@@ -6129,11 +6187,9 @@
         <v>579</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H8" s="30"/>
       <c r="I8" s="30"/>
       <c r="J8" s="31"/>
     </row>
@@ -6156,7 +6212,7 @@
         <v>26</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>726</v>
+        <v>889</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="31"/>
@@ -6180,7 +6236,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>726</v>
+        <v>888</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="31"/>
@@ -6204,7 +6260,7 @@
         <v>26</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>726</v>
+        <v>888</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="31"/>
@@ -6276,13 +6332,13 @@
         <v>26</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="32.25" thickBot="1">
@@ -6307,7 +6363,7 @@
       <c r="I15" s="30"/>
       <c r="J15" s="31"/>
     </row>
-    <row r="16" spans="1:10" ht="48" thickBot="1">
+    <row r="16" spans="1:10" ht="79.5" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>596</v>
       </c>
@@ -6328,7 +6384,7 @@
         <v>26</v>
       </c>
       <c r="H16" s="135" t="s">
-        <v>726</v>
+        <v>890</v>
       </c>
       <c r="I16" s="113"/>
       <c r="J16" s="114"/>
@@ -6359,7 +6415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -6428,11 +6484,11 @@
         <v>26</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="I2" s="50"/>
       <c r="J2" s="51" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
@@ -6476,11 +6532,11 @@
         <v>26</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="78.75">
@@ -6502,11 +6558,11 @@
         <v>26</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="48" thickBot="1">
@@ -6528,7 +6584,7 @@
         <v>26</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>794</v>
+        <v>708</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
@@ -6554,11 +6610,11 @@
         <v>26</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="I7" s="30"/>
       <c r="J7" s="121" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="79.5" thickBot="1">
@@ -6580,11 +6636,11 @@
         <v>26</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="121" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25">
@@ -6606,7 +6662,7 @@
         <v>26</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>794</v>
+        <v>708</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="31"/>
@@ -6652,11 +6708,11 @@
         <v>26</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="94.5">
@@ -6675,11 +6731,9 @@
         <v>622</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>794</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H12" s="30"/>
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
     </row>
@@ -6701,7 +6755,7 @@
         <v>625</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>690</v>
+        <v>56</v>
       </c>
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
@@ -6723,7 +6777,7 @@
         <v>627</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>690</v>
+        <v>56</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
@@ -6747,7 +6801,7 @@
         <v>630</v>
       </c>
       <c r="G15" s="30" t="s">
-        <v>690</v>
+        <v>56</v>
       </c>
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
@@ -6769,7 +6823,7 @@
         <v>632</v>
       </c>
       <c r="G16" s="113" t="s">
-        <v>690</v>
+        <v>56</v>
       </c>
       <c r="H16" s="113"/>
       <c r="I16" s="113"/>
@@ -6801,8 +6855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -6813,7 +6867,7 @@
     <col min="6" max="6" width="88.7109375" style="25" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="115" customWidth="1"/>
     <col min="8" max="8" width="35.28515625" style="115" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="115" customWidth="1"/>
+    <col min="9" max="9" width="45.42578125" style="115" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.42578125" style="115" customWidth="1"/>
     <col min="11" max="1024" width="8.85546875" style="25"/>
   </cols>
@@ -6869,16 +6923,16 @@
         <v>26</v>
       </c>
       <c r="H2" s="123" t="s">
-        <v>789</v>
+        <v>891</v>
       </c>
       <c r="I2" s="123" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="J2" s="124" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="63.75" thickBot="1">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="63.75" customHeight="1" thickBot="1">
       <c r="A3" s="140"/>
       <c r="B3" s="62" t="s">
         <v>636</v>
@@ -6897,16 +6951,16 @@
         <v>26</v>
       </c>
       <c r="H3" s="125" t="s">
-        <v>791</v>
+        <v>892</v>
       </c>
       <c r="I3" s="125" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="J3" s="126" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="63">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="32.25" thickBot="1">
       <c r="A4" s="140"/>
       <c r="B4" s="62" t="s">
         <v>638</v>
@@ -6925,13 +6979,13 @@
         <v>26</v>
       </c>
       <c r="H4" s="125" t="s">
-        <v>791</v>
+        <v>892</v>
       </c>
       <c r="I4" s="125" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="J4" s="126" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="47.25">
@@ -6951,13 +7005,13 @@
         <v>26</v>
       </c>
       <c r="H5" s="125" t="s">
-        <v>791</v>
+        <v>892</v>
       </c>
       <c r="I5" s="125" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="J5" s="126" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="94.5">
@@ -6977,13 +7031,13 @@
         <v>26</v>
       </c>
       <c r="H6" s="125" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="I6" s="125" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="J6" s="126" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="48" customHeight="1">
@@ -7007,16 +7061,16 @@
         <v>26</v>
       </c>
       <c r="H7" s="125" t="s">
+        <v>892</v>
+      </c>
+      <c r="I7" s="125" t="s">
+        <v>792</v>
+      </c>
+      <c r="J7" s="126" t="s">
         <v>791</v>
       </c>
-      <c r="I7" s="125" t="s">
-        <v>796</v>
-      </c>
-      <c r="J7" s="126" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="47.25">
+    </row>
+    <row r="8" spans="1:10" ht="31.5">
       <c r="A8" s="139"/>
       <c r="B8" s="62" t="s">
         <v>647</v>
@@ -7035,13 +7089,13 @@
         <v>26</v>
       </c>
       <c r="H8" s="125" t="s">
+        <v>892</v>
+      </c>
+      <c r="I8" s="125" t="s">
+        <v>800</v>
+      </c>
+      <c r="J8" s="126" t="s">
         <v>791</v>
-      </c>
-      <c r="I8" s="125" t="s">
-        <v>805</v>
-      </c>
-      <c r="J8" s="126" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25">
@@ -7085,13 +7139,13 @@
         <v>26</v>
       </c>
       <c r="H10" s="125" t="s">
+        <v>892</v>
+      </c>
+      <c r="I10" s="125" t="s">
+        <v>801</v>
+      </c>
+      <c r="J10" s="126" t="s">
         <v>791</v>
-      </c>
-      <c r="I10" s="125" t="s">
-        <v>806</v>
-      </c>
-      <c r="J10" s="126" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="31.5">
@@ -7176,11 +7230,9 @@
         <v>661</v>
       </c>
       <c r="G14" s="125" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="125" t="s">
-        <v>726</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H14" s="125"/>
       <c r="I14" s="125"/>
       <c r="J14" s="126"/>
     </row>
@@ -7203,9 +7255,11 @@
         <v>26</v>
       </c>
       <c r="H15" s="125" t="s">
-        <v>726</v>
-      </c>
-      <c r="I15" s="141"/>
+        <v>865</v>
+      </c>
+      <c r="I15" s="141" t="s">
+        <v>866</v>
+      </c>
       <c r="J15" s="126"/>
     </row>
     <row r="16" spans="1:10" ht="48" customHeight="1" thickBot="1">
@@ -7229,10 +7283,10 @@
         <v>26</v>
       </c>
       <c r="H16" s="125" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="I16" s="125" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="J16" s="126"/>
     </row>
@@ -7255,10 +7309,10 @@
         <v>26</v>
       </c>
       <c r="H17" s="125" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="I17" s="125" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="J17" s="126"/>
     </row>
@@ -7281,10 +7335,10 @@
         <v>26</v>
       </c>
       <c r="H18" s="125" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="I18" s="125" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="J18" s="126"/>
     </row>
@@ -7307,10 +7361,10 @@
         <v>26</v>
       </c>
       <c r="H19" s="125" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="I19" s="125" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="J19" s="126"/>
     </row>
@@ -7333,10 +7387,10 @@
         <v>26</v>
       </c>
       <c r="H20" s="125" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="I20" s="125" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="J20" s="126"/>
     </row>
@@ -7359,10 +7413,10 @@
         <v>26</v>
       </c>
       <c r="H21" s="125" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="I21" s="125" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="J21" s="126"/>
     </row>
@@ -7385,10 +7439,10 @@
         <v>26</v>
       </c>
       <c r="H22" s="125" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="I22" s="125" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="J22" s="126"/>
     </row>
@@ -7413,13 +7467,13 @@
         <v>26</v>
       </c>
       <c r="H23" s="125" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="I23" s="125" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="J23" s="126" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="31.5">
@@ -7441,13 +7495,13 @@
         <v>26</v>
       </c>
       <c r="H24" s="125" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="I24" s="125" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="J24" s="126" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="47.25">
@@ -7469,13 +7523,13 @@
         <v>26</v>
       </c>
       <c r="H25" s="125" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="I25" s="125" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="J25" s="126" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5">
@@ -7497,13 +7551,13 @@
         <v>26</v>
       </c>
       <c r="H26" s="127" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="I26" s="127" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="J26" s="128" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
     </row>
   </sheetData>
@@ -7533,8 +7587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -7546,7 +7600,7 @@
     <col min="6" max="6" width="60.85546875" style="15" customWidth="1"/>
     <col min="7" max="7" width="19.140625" style="38" customWidth="1"/>
     <col min="8" max="8" width="38.42578125" style="38" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="38" customWidth="1"/>
+    <col min="9" max="9" width="39" style="38" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41.7109375" style="38" customWidth="1"/>
     <col min="11" max="1024" width="8.85546875" style="15"/>
   </cols>
@@ -7602,10 +7656,10 @@
         <v>26</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>828</v>
+        <v>821</v>
       </c>
       <c r="J2" s="24"/>
     </row>
@@ -7628,10 +7682,10 @@
         <v>26</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>835</v>
+        <v>828</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>689</v>
@@ -7656,10 +7710,10 @@
         <v>26</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>830</v>
+        <v>823</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>831</v>
+        <v>824</v>
       </c>
       <c r="J4" s="31"/>
     </row>
@@ -7682,10 +7736,10 @@
         <v>26</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>834</v>
+        <v>827</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>836</v>
+        <v>829</v>
       </c>
       <c r="J5" s="31" t="s">
         <v>689</v>
@@ -7710,10 +7764,10 @@
         <v>26</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>840</v>
+        <v>833</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>841</v>
+        <v>834</v>
       </c>
       <c r="J6" s="31" t="s">
         <v>689</v>
@@ -7760,10 +7814,10 @@
         <v>26</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>843</v>
+        <v>836</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>844</v>
+        <v>837</v>
       </c>
       <c r="J8" s="31"/>
     </row>
@@ -7788,10 +7842,10 @@
         <v>26</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>845</v>
+        <v>838</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="J9" s="31"/>
     </row>
@@ -7817,10 +7871,10 @@
         <v>708</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="25" customFormat="1" ht="63">
@@ -7845,10 +7899,10 @@
         <v>708</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="25" customFormat="1" ht="63">
@@ -7915,10 +7969,10 @@
         <v>708</v>
       </c>
       <c r="I14" s="133" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="J14" s="137" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="25" customFormat="1" ht="15.75">
@@ -7987,10 +8041,10 @@
         <v>708</v>
       </c>
       <c r="I17" s="30" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="25" customFormat="1" ht="94.5">
@@ -8015,10 +8069,10 @@
         <v>708</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
@@ -8042,13 +8096,13 @@
         <v>26</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="25" customFormat="1" ht="78.75">
@@ -8070,13 +8124,13 @@
         <v>26</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="25" customFormat="1" ht="47.25">
@@ -8101,10 +8155,10 @@
         <v>691</v>
       </c>
       <c r="I21" s="30" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="J21" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="25" customFormat="1" ht="63">
@@ -8126,10 +8180,10 @@
         <v>26</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>801</v>
+        <v>865</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>801</v>
+        <v>867</v>
       </c>
       <c r="J22" s="31"/>
     </row>
@@ -8198,10 +8252,10 @@
         <v>26</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>801</v>
+        <v>709</v>
       </c>
       <c r="I25" s="30" t="s">
-        <v>801</v>
+        <v>868</v>
       </c>
       <c r="J25" s="31"/>
     </row>
@@ -8224,13 +8278,13 @@
         <v>26</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
@@ -8257,10 +8311,10 @@
         <v>708</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="J27" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="25" customFormat="1" ht="63">
@@ -8277,14 +8331,10 @@
         <v>90</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>801</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>801</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
       <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" s="25" customFormat="1" ht="32.25" customHeight="1">
@@ -8306,16 +8356,16 @@
         <v>26</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="I29" s="30" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="J29" s="31" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="25" customFormat="1" ht="78.75">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="25" customFormat="1" ht="94.5">
       <c r="A30" s="138"/>
       <c r="B30" s="19" t="s">
         <v>94</v>
@@ -8332,10 +8382,10 @@
         <v>26</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>801</v>
+        <v>869</v>
       </c>
       <c r="I30" s="30" t="s">
-        <v>801</v>
+        <v>870</v>
       </c>
       <c r="J30" s="31"/>
     </row>
@@ -8360,10 +8410,10 @@
         <v>26</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="I31" s="30" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="J31" s="31"/>
     </row>
@@ -8386,10 +8436,10 @@
         <v>26</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>801</v>
+        <v>871</v>
       </c>
       <c r="I32" s="30" t="s">
-        <v>801</v>
+        <v>872</v>
       </c>
       <c r="J32" s="31"/>
     </row>
@@ -8415,10 +8465,10 @@
       </c>
       <c r="H33" s="30"/>
       <c r="I33" s="30" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
@@ -8442,7 +8492,7 @@
         <v>26</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="I34" s="30" t="s">
         <v>688</v>
@@ -8468,7 +8518,7 @@
         <v>26</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="I35" s="30"/>
       <c r="J35" s="31"/>
@@ -8492,7 +8542,7 @@
         <v>26</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="I36" s="30"/>
       <c r="J36" s="31"/>
@@ -8582,13 +8632,13 @@
         <v>26</v>
       </c>
       <c r="H40" s="133" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="I40" s="133" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="J40" s="137" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="25" customFormat="1" ht="63">
@@ -8610,13 +8660,13 @@
         <v>26</v>
       </c>
       <c r="H41" s="133" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="I41" s="30" t="s">
-        <v>858</v>
+        <v>851</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>859</v>
+        <v>852</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="25" customFormat="1" ht="78.75">
@@ -8638,13 +8688,13 @@
         <v>26</v>
       </c>
       <c r="H42" s="133" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="I42" s="30" t="s">
-        <v>860</v>
+        <v>853</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>861</v>
+        <v>854</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="25" customFormat="1" ht="78.75">
@@ -8664,13 +8714,13 @@
         <v>26</v>
       </c>
       <c r="H43" s="133" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="I43" s="133" t="s">
-        <v>862</v>
+        <v>855</v>
       </c>
       <c r="J43" s="137" t="s">
-        <v>863</v>
+        <v>856</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="25" customFormat="1" ht="94.5">
@@ -8692,13 +8742,13 @@
         <v>26</v>
       </c>
       <c r="H44" s="133" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="I44" s="30" t="s">
-        <v>865</v>
+        <v>858</v>
       </c>
       <c r="J44" s="137" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="25" customFormat="1" ht="63">
@@ -8717,27 +8767,25 @@
         <v>129</v>
       </c>
       <c r="G45" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="H45" s="113" t="s">
-        <v>801</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H45" s="113"/>
       <c r="I45" s="113"/>
       <c r="J45" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8758,8 +8806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50:I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -8948,11 +8996,9 @@
         <v>141</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
     </row>
@@ -8974,11 +9020,9 @@
         <v>143</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="133" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H7" s="133"/>
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
     </row>
@@ -9000,11 +9044,9 @@
         <v>145</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="133" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H8" s="133"/>
       <c r="I8" s="30"/>
       <c r="J8" s="31"/>
     </row>
@@ -9026,11 +9068,9 @@
         <v>147</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="133" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H9" s="133"/>
       <c r="I9" s="30"/>
       <c r="J9" s="31"/>
     </row>
@@ -9082,11 +9122,9 @@
         <v>151</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="133" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H11" s="133"/>
       <c r="I11" s="30"/>
       <c r="J11" s="31"/>
     </row>
@@ -9108,11 +9146,9 @@
         <v>153</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="133" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H12" s="133"/>
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
     </row>
@@ -9134,11 +9170,9 @@
         <v>155</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="133" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H13" s="133"/>
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
     </row>
@@ -9189,9 +9223,11 @@
         <v>26</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="I15" s="30"/>
+        <v>875</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>874</v>
+      </c>
       <c r="J15" s="31"/>
     </row>
     <row r="16" spans="1:10" s="25" customFormat="1" ht="95.25" thickBot="1">
@@ -9288,7 +9324,7 @@
       <c r="I19" s="30"/>
       <c r="J19" s="31"/>
     </row>
-    <row r="20" spans="1:10" s="25" customFormat="1" ht="32.25" thickBot="1">
+    <row r="20" spans="1:10" s="25" customFormat="1" ht="48" thickBot="1">
       <c r="A20" s="139"/>
       <c r="B20" s="44" t="s">
         <v>174</v>
@@ -9309,9 +9345,11 @@
         <v>26</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="I20" s="30"/>
+        <v>875</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>874</v>
+      </c>
       <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10" s="25" customFormat="1" ht="79.5" customHeight="1" thickBot="1">
@@ -9334,7 +9372,7 @@
         <v>180</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>690</v>
+        <v>56</v>
       </c>
       <c r="H21" s="30"/>
       <c r="I21" s="30"/>
@@ -9358,7 +9396,7 @@
         <v>183</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>690</v>
+        <v>26</v>
       </c>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
@@ -9382,7 +9420,7 @@
         <v>186</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>690</v>
+        <v>56</v>
       </c>
       <c r="H23" s="30"/>
       <c r="I23" s="30"/>
@@ -9509,7 +9547,7 @@
         <v>26</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="I28" s="30"/>
       <c r="J28" s="31"/>
@@ -9534,11 +9572,9 @@
         <v>200</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H29" s="30"/>
       <c r="I29" s="30"/>
       <c r="J29" s="31"/>
     </row>
@@ -9560,11 +9596,9 @@
         <v>202</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H30" s="30"/>
       <c r="I30" s="30"/>
       <c r="J30" s="31"/>
     </row>
@@ -9586,11 +9620,9 @@
         <v>204</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H31" s="30"/>
       <c r="I31" s="30"/>
       <c r="J31" s="31"/>
     </row>
@@ -9612,11 +9644,9 @@
         <v>206</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H32" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H32" s="30"/>
       <c r="I32" s="30"/>
       <c r="J32" s="31"/>
     </row>
@@ -9638,11 +9668,9 @@
         <v>209</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H33" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H33" s="30"/>
       <c r="I33" s="30"/>
       <c r="J33" s="31"/>
     </row>
@@ -9664,11 +9692,9 @@
         <v>211</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H34" s="30"/>
       <c r="I34" s="30"/>
       <c r="J34" s="31"/>
     </row>
@@ -9690,11 +9716,9 @@
         <v>213</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H35" s="30"/>
       <c r="I35" s="30"/>
       <c r="J35" s="31"/>
     </row>
@@ -9945,10 +9969,10 @@
         <v>26</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>726</v>
+        <v>875</v>
       </c>
       <c r="I45" s="30" t="s">
-        <v>726</v>
+        <v>874</v>
       </c>
       <c r="J45" s="31"/>
     </row>
@@ -9973,14 +9997,14 @@
         <v>26</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>726</v>
+        <v>875</v>
       </c>
       <c r="I46" s="30" t="s">
-        <v>726</v>
+        <v>874</v>
       </c>
       <c r="J46" s="31"/>
     </row>
-    <row r="47" spans="1:10" s="25" customFormat="1" ht="32.25" thickBot="1">
+    <row r="47" spans="1:10" s="25" customFormat="1" ht="48" thickBot="1">
       <c r="A47" s="139"/>
       <c r="B47" s="44" t="s">
         <v>242</v>
@@ -10001,14 +10025,14 @@
         <v>26</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>726</v>
+        <v>875</v>
       </c>
       <c r="I47" s="30" t="s">
-        <v>726</v>
+        <v>874</v>
       </c>
       <c r="J47" s="31"/>
     </row>
-    <row r="48" spans="1:10" s="25" customFormat="1" ht="32.25" thickBot="1">
+    <row r="48" spans="1:10" s="25" customFormat="1" ht="48" thickBot="1">
       <c r="A48" s="139"/>
       <c r="B48" s="44" t="s">
         <v>244</v>
@@ -10029,10 +10053,10 @@
         <v>26</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>726</v>
+        <v>875</v>
       </c>
       <c r="I48" s="30" t="s">
-        <v>726</v>
+        <v>874</v>
       </c>
       <c r="J48" s="31"/>
     </row>
@@ -10057,10 +10081,10 @@
         <v>26</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>726</v>
+        <v>875</v>
       </c>
       <c r="I49" s="30" t="s">
-        <v>726</v>
+        <v>874</v>
       </c>
       <c r="J49" s="31"/>
     </row>
@@ -10085,10 +10109,10 @@
         <v>26</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>726</v>
+        <v>875</v>
       </c>
       <c r="I50" s="30" t="s">
-        <v>726</v>
+        <v>874</v>
       </c>
       <c r="J50" s="31"/>
     </row>
@@ -10110,14 +10134,10 @@
         <v>254</v>
       </c>
       <c r="G51" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H51" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="I51" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
       <c r="J51" s="31"/>
     </row>
     <row r="52" spans="1:10" s="25" customFormat="1" ht="63.75" customHeight="1" thickBot="1">
@@ -10143,11 +10163,11 @@
         <v>26</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I52" s="30"/>
       <c r="J52" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="25" customFormat="1" ht="48" thickBot="1">
@@ -10171,11 +10191,11 @@
         <v>26</v>
       </c>
       <c r="H53" s="30" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I53" s="30"/>
       <c r="J53" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="25" customFormat="1" ht="48" thickBot="1">
@@ -10199,11 +10219,11 @@
         <v>26</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I54" s="30"/>
       <c r="J54" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="25" customFormat="1" ht="79.5" customHeight="1" thickBot="1">
@@ -10235,7 +10255,7 @@
         <v>725</v>
       </c>
       <c r="J55" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="25" customFormat="1" ht="48" thickBot="1">
@@ -10259,7 +10279,7 @@
         <v>26</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I56" s="30"/>
       <c r="J56" s="31" t="s">
@@ -10293,7 +10313,7 @@
         <v>725</v>
       </c>
       <c r="J57" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="25" customFormat="1" ht="95.25" thickBot="1">
@@ -10315,10 +10335,10 @@
         <v>26</v>
       </c>
       <c r="H58" s="122" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="I58" s="113" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="J58" s="114" t="s">
         <v>714</v>
@@ -10326,16 +10346,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A55:A58"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A55:A58"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -10356,7 +10376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -10581,7 +10601,7 @@
         <v>26</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I7" s="30" t="s">
         <v>717</v>
@@ -10611,10 +10631,10 @@
         <v>26</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J8" s="121" t="s">
         <v>718</v>
@@ -10639,10 +10659,10 @@
         <v>26</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J9" s="121" t="s">
         <v>718</v>
@@ -10845,7 +10865,7 @@
         <v>26</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I17" s="30"/>
       <c r="J17" s="121" t="s">
@@ -10871,7 +10891,7 @@
         <v>26</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="I18" s="30"/>
       <c r="J18" s="121" t="s">
@@ -10952,7 +10972,7 @@
         <v>708</v>
       </c>
       <c r="I21" s="113" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="J21" s="114" t="s">
         <v>718</v>
@@ -11006,8 +11026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -11080,7 +11100,7 @@
         <v>708</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="J2" s="51" t="s">
         <v>714</v>
@@ -11108,7 +11128,7 @@
         <v>708</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>714</v>
@@ -11136,7 +11156,7 @@
         <v>708</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="J4" s="31" t="s">
         <v>714</v>
@@ -11186,7 +11206,7 @@
         <v>708</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J6" s="31" t="s">
         <v>714</v>
@@ -11216,7 +11236,7 @@
         <v>708</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J7" s="31" t="s">
         <v>714</v>
@@ -11244,7 +11264,7 @@
         <v>708</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J8" s="31" t="s">
         <v>714</v>
@@ -11271,9 +11291,11 @@
         <v>26</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>748</v>
-      </c>
-      <c r="I9" s="30"/>
+        <v>875</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>874</v>
+      </c>
       <c r="J9" s="31"/>
     </row>
     <row r="10" spans="1:10" ht="63.75" thickBot="1">
@@ -11294,9 +11316,7 @@
       <c r="G10" s="30" t="s">
         <v>690</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>748</v>
-      </c>
+      <c r="H10" s="30"/>
       <c r="I10" s="30"/>
       <c r="J10" s="31"/>
     </row>
@@ -11322,7 +11342,7 @@
         <v>707</v>
       </c>
       <c r="I11" s="113" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J11" s="114" t="s">
         <v>718</v>
@@ -11353,8 +11373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -11423,10 +11443,10 @@
         <v>26</v>
       </c>
       <c r="H2" s="50" t="s">
+        <v>742</v>
+      </c>
+      <c r="I2" s="50" t="s">
         <v>743</v>
-      </c>
-      <c r="I2" s="50" t="s">
-        <v>744</v>
       </c>
       <c r="J2" s="119" t="s">
         <v>714</v>
@@ -11451,13 +11471,13 @@
         <v>26</v>
       </c>
       <c r="H3" s="30" t="s">
+        <v>776</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>777</v>
+      </c>
+      <c r="J3" s="31" t="s">
         <v>778</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>779</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="79.5" thickBot="1">
@@ -11482,10 +11502,10 @@
         <v>691</v>
       </c>
       <c r="I4" s="30" t="s">
+        <v>744</v>
+      </c>
+      <c r="J4" s="31" t="s">
         <v>745</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="111" thickBot="1">
@@ -11507,13 +11527,13 @@
         <v>26</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="48" thickBot="1">
@@ -11538,10 +11558,10 @@
         <v>708</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="63.75" customHeight="1" thickBot="1">
@@ -11596,10 +11616,10 @@
         <v>691</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="48" thickBot="1">
@@ -11764,10 +11784,10 @@
         <v>691</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="126.75" customHeight="1" thickBot="1">
@@ -11791,12 +11811,14 @@
         <v>26</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>801</v>
+        <v>691</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>801</v>
-      </c>
-      <c r="J15" s="31"/>
+        <v>876</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="79.5" thickBot="1">
       <c r="A16" s="139"/>
@@ -11814,14 +11836,10 @@
         <v>373</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>801</v>
-      </c>
-      <c r="I16" s="30" t="s">
-        <v>801</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
       <c r="J16" s="31"/>
     </row>
     <row r="17" spans="1:11" ht="63.75" thickBot="1">
@@ -11865,13 +11883,13 @@
         <v>26</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>823</v>
+        <v>816</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>824</v>
+        <v>817</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="95.25" thickBot="1">
@@ -11890,14 +11908,10 @@
         <v>379</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>801</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>801</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
       <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:11" ht="63.75" thickBot="1">
@@ -11916,14 +11930,10 @@
         <v>381</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="30" t="s">
-        <v>801</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>801</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
       <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:11" ht="79.5" thickBot="1">
@@ -12008,14 +12018,10 @@
         <v>389</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24" s="30" t="s">
-        <v>801</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>801</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
       <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:11" ht="48" customHeight="1" thickBot="1">
@@ -12039,12 +12045,14 @@
         <v>26</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>801</v>
+        <v>877</v>
       </c>
       <c r="I25" s="30" t="s">
-        <v>801</v>
-      </c>
-      <c r="J25" s="31"/>
+        <v>879</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="32.25" thickBot="1">
       <c r="A26" s="139"/>
@@ -12065,13 +12073,13 @@
         <v>26</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="32.25" thickBot="1">
@@ -12093,13 +12101,13 @@
         <v>26</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="J27" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="95.25" thickBot="1">
@@ -12244,7 +12252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -12315,13 +12323,13 @@
         <v>26</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="47.25">
@@ -12343,13 +12351,13 @@
         <v>26</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="47.25">
@@ -12371,13 +12379,13 @@
         <v>26</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="32.25" customHeight="1">
@@ -12401,13 +12409,13 @@
         <v>26</v>
       </c>
       <c r="H5" s="30" t="s">
+        <v>749</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>750</v>
+      </c>
+      <c r="J5" s="31" t="s">
         <v>751</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>752</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="48" thickBot="1">
@@ -12432,10 +12440,10 @@
         <v>720</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="32.25" thickBot="1">
@@ -12460,10 +12468,10 @@
         <v>720</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="48" thickBot="1">
@@ -12488,10 +12496,10 @@
         <v>720</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="48" thickBot="1">
@@ -12516,10 +12524,10 @@
         <v>720</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="48" thickBot="1">
@@ -12544,10 +12552,10 @@
         <v>720</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="32.25" thickBot="1">
@@ -12572,10 +12580,10 @@
         <v>720</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="31.5">
@@ -12600,10 +12608,10 @@
         <v>720</v>
       </c>
       <c r="I12" s="30" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1">
@@ -12627,13 +12635,13 @@
         <v>26</v>
       </c>
       <c r="H13" s="30" t="s">
+        <v>762</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>763</v>
+      </c>
+      <c r="J13" s="31" t="s">
         <v>764</v>
-      </c>
-      <c r="I13" s="30" t="s">
-        <v>765</v>
-      </c>
-      <c r="J13" s="31" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="47.25">
@@ -12655,13 +12663,13 @@
         <v>26</v>
       </c>
       <c r="H14" s="30" t="s">
+        <v>762</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>763</v>
+      </c>
+      <c r="J14" s="31" t="s">
         <v>764</v>
-      </c>
-      <c r="I14" s="30" t="s">
-        <v>765</v>
-      </c>
-      <c r="J14" s="31" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="31.5">
@@ -12683,13 +12691,13 @@
         <v>26</v>
       </c>
       <c r="H15" s="30" t="s">
+        <v>762</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>763</v>
+      </c>
+      <c r="J15" s="31" t="s">
         <v>764</v>
-      </c>
-      <c r="I15" s="30" t="s">
-        <v>765</v>
-      </c>
-      <c r="J15" s="31" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="48" customHeight="1">
@@ -12719,7 +12727,7 @@
         <v>725</v>
       </c>
       <c r="J16" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="78.75">
@@ -12741,13 +12749,13 @@
         <v>26</v>
       </c>
       <c r="H17" s="113" t="s">
+        <v>769</v>
+      </c>
+      <c r="I17" s="113" t="s">
         <v>771</v>
       </c>
-      <c r="I17" s="113" t="s">
-        <v>773</v>
-      </c>
       <c r="J17" s="114" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
   </sheetData>
@@ -12776,8 +12784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -12847,7 +12855,7 @@
         <v>26</v>
       </c>
       <c r="H2" s="117" t="s">
-        <v>748</v>
+        <v>880</v>
       </c>
       <c r="I2" s="117"/>
       <c r="J2" s="118"/>
@@ -12871,7 +12879,7 @@
         <v>26</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>748</v>
+        <v>880</v>
       </c>
       <c r="I3" s="30"/>
       <c r="J3" s="31"/>
@@ -12895,7 +12903,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>748</v>
+        <v>880</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
@@ -12919,7 +12927,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>748</v>
+        <v>880</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
@@ -12945,7 +12953,7 @@
         <v>26</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>748</v>
+        <v>880</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
@@ -12969,7 +12977,7 @@
         <v>26</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>748</v>
+        <v>880</v>
       </c>
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
@@ -12995,13 +13003,13 @@
         <v>26</v>
       </c>
       <c r="H8" s="30" t="s">
+        <v>765</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>766</v>
+      </c>
+      <c r="J8" s="31" t="s">
         <v>767</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>768</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" thickBot="1">
@@ -13026,7 +13034,7 @@
       <c r="I9" s="30"/>
       <c r="J9" s="31"/>
     </row>
-    <row r="10" spans="1:10" ht="48" thickBot="1">
+    <row r="10" spans="1:10" ht="48" customHeight="1" thickBot="1">
       <c r="A10" s="139"/>
       <c r="B10" s="62" t="s">
         <v>457</v>
@@ -13044,10 +13052,10 @@
       <c r="G10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>748</v>
-      </c>
-      <c r="I10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30" t="s">
+        <v>881</v>
+      </c>
       <c r="J10" s="31"/>
     </row>
     <row r="11" spans="1:10" ht="63.75" thickBot="1">
@@ -13122,7 +13130,7 @@
         <v>708</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="J13" s="31" t="s">
         <v>714</v>
@@ -13146,8 +13154,8 @@
       <c r="G14" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="113" t="s">
-        <v>748</v>
+      <c r="H14" s="135" t="s">
+        <v>708</v>
       </c>
       <c r="I14" s="113"/>
       <c r="J14" s="114"/>
@@ -13178,7 +13186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -13248,13 +13256,13 @@
         <v>26</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="47.25">
@@ -13275,8 +13283,8 @@
       <c r="G3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="30" t="s">
-        <v>726</v>
+      <c r="H3" s="133" t="s">
+        <v>859</v>
       </c>
       <c r="I3" s="30"/>
       <c r="J3" s="31"/>
@@ -13300,13 +13308,13 @@
         <v>26</v>
       </c>
       <c r="H4" s="30" t="s">
+        <v>772</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>773</v>
+      </c>
+      <c r="J4" s="31" t="s">
         <v>774</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>775</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="31.5">
@@ -13328,13 +13336,13 @@
         <v>26</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="31.5">
@@ -13353,11 +13361,9 @@
         <v>478</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
     </row>
@@ -13377,11 +13383,9 @@
         <v>480</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H7" s="30"/>
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
     </row>
@@ -13405,10 +13409,10 @@
       <c r="G8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="I8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30" t="s">
+        <v>882</v>
+      </c>
       <c r="J8" s="31"/>
     </row>
     <row r="9" spans="1:10" ht="31.5">
@@ -13429,10 +13433,10 @@
       <c r="G9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="I9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30" t="s">
+        <v>882</v>
+      </c>
       <c r="J9" s="31"/>
     </row>
     <row r="10" spans="1:10" ht="31.5">
@@ -13453,10 +13457,10 @@
       <c r="G10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="I10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30" t="s">
+        <v>882</v>
+      </c>
       <c r="J10" s="31"/>
     </row>
     <row r="11" spans="1:10" ht="32.25" customHeight="1">
@@ -13505,7 +13509,7 @@
       </c>
       <c r="H12" s="30"/>
       <c r="I12" s="30" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
       <c r="J12" s="31"/>
     </row>
@@ -13525,11 +13529,9 @@
         <v>494</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>726</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="H13" s="30"/>
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
     </row>
@@ -13551,10 +13553,10 @@
       <c r="G14" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="I14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30" t="s">
+        <v>883</v>
+      </c>
       <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:10" ht="31.5">
@@ -13576,7 +13578,7 @@
         <v>26</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>726</v>
+        <v>880</v>
       </c>
       <c r="I15" s="30"/>
       <c r="J15" s="31"/>
@@ -13599,10 +13601,10 @@
       <c r="G16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="I16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30" t="s">
+        <v>884</v>
+      </c>
       <c r="J16" s="31"/>
     </row>
     <row r="17" spans="1:10" ht="48" thickBot="1">
@@ -13624,10 +13626,12 @@
         <v>26</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>726</v>
+        <v>749</v>
       </c>
       <c r="I17" s="30"/>
-      <c r="J17" s="31"/>
+      <c r="J17" s="137" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="32.25" thickBot="1">
       <c r="A18" s="139"/>
@@ -13645,11 +13649,9 @@
         <v>504</v>
       </c>
       <c r="G18" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="135" t="s">
-        <v>726</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H18" s="135"/>
       <c r="I18" s="113"/>
       <c r="J18" s="114"/>
     </row>
@@ -13675,15 +13677,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="caec8013-4252-46d5-9263-a99cc59dead2">
@@ -13692,6 +13685,15 @@
     <TaxCatchAll xmlns="d77a0e16-36e2-4619-a824-6737dea303d4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13924,26 +13926,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1115CF8-E078-4757-AB4D-549A55AF833E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB94848C-75E5-4594-8307-209BB5BE433B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="d77a0e16-36e2-4619-a824-6737dea303d4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="caec8013-4252-46d5-9263-a99cc59dead2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB94848C-75E5-4594-8307-209BB5BE433B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1115CF8-E078-4757-AB4D-549A55AF833E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="caec8013-4252-46d5-9263-a99cc59dead2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="d77a0e16-36e2-4619-a824-6737dea303d4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>